<commit_message>
Permission set to local, updates to file
</commit_message>
<xml_diff>
--- a/CLASSOPS/Jeannine/Jeannine's log.xlsx
+++ b/CLASSOPS/Jeannine/Jeannine's log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="180">
   <si>
     <t>Staff Name</t>
   </si>
@@ -547,6 +547,21 @@
   </si>
   <si>
     <t>121</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Demo neck mic and PC</t>
+  </si>
+  <si>
+    <t>1850</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demo neck mic and PC </t>
   </si>
 </sst>
 </file>
@@ -1065,9 +1080,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F139" sqref="F139"/>
     </sheetView>
   </sheetViews>
@@ -2692,6 +2707,56 @@
       </c>
       <c r="E133" s="11" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="21"/>
+      <c r="B137" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C137" s="23"/>
+      <c r="D137" s="21"/>
+      <c r="E137" s="24"/>
+      <c r="F137" s="25"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B138" s="10">
+        <v>42621</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D138" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E138" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F138" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B139" s="10">
+        <v>42621</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D139" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E139" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F139" s="19" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on a setting window
</commit_message>
<xml_diff>
--- a/CLASSOPS/Jeannine/Jeannine's log.xlsx
+++ b/CLASSOPS/Jeannine/Jeannine's log.xlsx
@@ -561,7 +561,7 @@
     <t>I</t>
   </si>
   <si>
-    <t xml:space="preserve">Demo neck mic and PC </t>
+    <t>Demo neck  mic and PC - please demo log off for PC and touchscreen. Please tell prof to put neck mic back in podium drawer (on right hand side of podium) at end of class and shut cabinet tightly as no one will be there for 10:00 pm log off.</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1083,7 @@
   <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F139" sqref="F139"/>
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,7 +2739,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Files updated, All message boxes were updated to Metro style. Metro UI updated to v1.4. minor bug fixes.
</commit_message>
<xml_diff>
--- a/CLASSOPS/Jeannine/Jeannine's log.xlsx
+++ b/CLASSOPS/Jeannine/Jeannine's log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="249">
   <si>
     <t>Staff Name</t>
   </si>
@@ -742,6 +742,33 @@
   </si>
   <si>
     <t>Wardha</t>
+  </si>
+  <si>
+    <t>Please demo equipment to client and make sure client is happy.</t>
+  </si>
+  <si>
+    <t>Make sure neck mic goes back to drawer and log off touchscreen.</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>NO CEILING PROJECTOR - Use roll in PC and Projector that is in room. Make sure client is okay.</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>PLEASE LOCK ROOM. ALLEN KEY (with yellow handle) and CLH key is on keyrack in Lassonde 1011 office. PLEASE LOCK ALL 4 DOORS.</t>
+  </si>
+  <si>
+    <t>2130</t>
+  </si>
+  <si>
+    <t>LEAVE ROLL IN PC AND PROJECTOR IN ROOM - JUST TURN OFF. PLEASE LOCK ROOM. ALLEN KEY (with yellow handle) and CLH key is on keyrack in Lasonde 1011 office. PLEASE LOCK ALL 4 DOORS.</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -1260,10 +1287,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F255"/>
+  <dimension ref="A1:F269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E259" sqref="E259"/>
+    <sheetView tabSelected="1" topLeftCell="A254" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F272" sqref="F272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4510,6 +4537,216 @@
       </c>
       <c r="F255" s="19" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" s="21"/>
+      <c r="B259" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C259" s="23"/>
+      <c r="D259" s="21"/>
+      <c r="E259" s="24"/>
+      <c r="F259" s="25"/>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B260" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C260" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D260" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E260" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F260" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B261" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C261" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D261" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E261" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F261" s="19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B262" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C262" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D262" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E262" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F262" s="19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B263" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C263" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D263" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E263" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F263" s="19" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A264" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B264" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C264" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D264" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E264" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F264" s="19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A265" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B265" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C265" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D265" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E265" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F265" s="19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A266" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B266" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C266" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D266" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E266" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F266" s="19" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A267" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B267" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C267" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="D267" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E267" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F267" s="19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A268" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B268" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C268" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D268" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E268" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F268" s="19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A269" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B269" s="10">
+        <v>42640</v>
+      </c>
+      <c r="C269" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D269" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E269" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F269" s="19" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for release on version 0.2.9
</commit_message>
<xml_diff>
--- a/CLASSOPS/Jeannine/Jeannine's log.xlsx
+++ b/CLASSOPS/Jeannine/Jeannine's log.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1910" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="271">
   <si>
     <t>Staff Name</t>
   </si>
@@ -1362,10 +1362,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F538"/>
+  <dimension ref="A1:F558"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A522" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F543" sqref="F543"/>
+    <sheetView tabSelected="1" topLeftCell="A549" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F563" sqref="F563"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8831,6 +8831,336 @@
         <v>121</v>
       </c>
       <c r="F538" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A542" s="21"/>
+      <c r="B542" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C542" s="23"/>
+      <c r="D542" s="21"/>
+      <c r="E542" s="24"/>
+      <c r="F542" s="25"/>
+    </row>
+    <row r="543" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A543" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B543" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C543" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D543" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E543" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F543" s="19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="544" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A544" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B544" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C544" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D544" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E544" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F544" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="545" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A545" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B545" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C545" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D545" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E545" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F545" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="546" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A546" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B546" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C546" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D546" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E546" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F546" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="547" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A547" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B547" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C547" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D547" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E547" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F547" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A548" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B548" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C548" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D548" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E548" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F548" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A549" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B549" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C549" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D549" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E549" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F549" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A550" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B550" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C550" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D550" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E550" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F550" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="551" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A551" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B551" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C551" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D551" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E551" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F551" s="19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A552" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B552" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C552" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D552" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E552" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F552" s="19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A553" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B553" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C553" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D553" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E553" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F553" s="19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A554" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B554" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C554" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D554" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E554" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F554" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A555" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B555" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C555" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D555" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E555" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F555" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A556" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B556" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C556" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D556" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E556" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F556" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A557" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B557" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C557" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D557" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E557" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F557" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A558" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B558" s="10">
+        <v>42669</v>
+      </c>
+      <c r="C558" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D558" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E558" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F558" s="19" t="s">
         <v>244</v>
       </c>
     </row>

</xml_diff>